<commit_message>
Update by John on Task 2.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -40,7 +40,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +57,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ADD8E6"/>
         <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF6347"/>
+        <bgColor rgb="00FF6347"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -101,6 +107,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,6 +487,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2962275" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1051,6 +1087,16 @@
           <t>John</t>
         </is>
       </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-04 09:35:40</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1231,7 +1277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1291,6 +1337,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1312,6 +1372,79 @@
       <c r="B21" s="6" t="inlineStr">
         <is>
           <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Task 2.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Dashboard &gt; Logout &gt; Button</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 09:35:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>Failed</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1495,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1395,7 +1528,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2.1</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1552,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 09:32:17</t>
+          <t>2025-05-04 09:35:40</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1564,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[█-------------------] 5%</t>
+          <t>[██------------------] 11%</t>
         </is>
       </c>
     </row>
@@ -1454,7 +1587,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1476,7 +1609,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update by Paul on Task 3.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Task ID 2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -395,12 +396,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40</f>
+              <f>'Summary'!$A$40:$A$41</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40</f>
+              <f>'Summary'!$B$40:$B$41</f>
             </numRef>
           </val>
         </ser>
@@ -521,6 +522,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -594,6 +598,36 @@
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
     <clientData/>
   </oneCellAnchor>
 </wsDr>
@@ -1124,6 +1158,16 @@
           <t>Paul</t>
         </is>
       </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-05-04 09:35:52</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1337,20 +1381,6 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1460,7 +1490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1495,7 +1525,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1528,7 +1558,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>3.0</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1570,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Paul</t>
         </is>
       </c>
     </row>
@@ -1552,7 +1582,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 09:35:40</t>
+          <t>2025-05-04 09:35:52</t>
         </is>
       </c>
     </row>
@@ -1564,7 +1594,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[██------------------] 11%</t>
+          <t>[███-----------------] 16%</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1617,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1610,6 +1640,112 @@
       </c>
       <c r="B40" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Task 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Home &gt; Dashboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 09:35:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>TEst</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update by John on Task 2.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Task ID 3" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Task ID 2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -40,7 +41,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +58,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ADD8E6"/>
         <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -101,6 +108,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,12 +396,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40</f>
+              <f>'Summary'!$A$40:$A$41</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40</f>
+              <f>'Summary'!$B$40:$B$41</f>
             </numRef>
           </val>
         </ser>
@@ -485,6 +494,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -558,6 +570,36 @@
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
     <clientData/>
   </oneCellAnchor>
 </wsDr>
@@ -1014,6 +1056,16 @@
           <t>John</t>
         </is>
       </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-05-04 10:16:16</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1327,7 +1379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1352,7 +1404,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1383,7 +1435,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>5.56%</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1447,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1459,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>John</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1471,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 09:42:46</t>
+          <t>2025-05-04 10:16:16</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1483,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[█-------------------] 5%</t>
+          <t>[██------------------] 11%</t>
         </is>
       </c>
     </row>
@@ -1454,7 +1506,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1472,11 +1524,117 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Task 2.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Dashboard &gt; Settings &gt; Logout</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 10:16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Test1 - Ashish</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update by Paul on Task 3.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -501,6 +501,31 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -598,6 +623,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1155,6 +1183,16 @@
           <t>Paul</t>
         </is>
       </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-05-04 10:17:01</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1283,7 +1321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1343,6 +1381,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1364,6 +1416,79 @@
       <c r="B21" s="6" t="inlineStr">
         <is>
           <t>hold</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Task 3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Home &gt; check &gt; username </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 10:17:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>Test2 - Ashish</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1529,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1435,7 +1560,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5.56%</t>
+          <t>11.11%</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1572,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.1</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1584,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Paul</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1596,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 10:16:16</t>
+          <t>2025-05-04 10:17:01</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1608,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[██------------------] 11%</t>
+          <t>[███-----------------] 16%</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1631,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1524,17 +1649,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B41" t="n">

</xml_diff>

<commit_message>
Update by Vaishnavi on Task 1.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Task ID 3" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Task ID 2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Task ID 1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -41,7 +42,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -64,6 +65,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="0090EE90"/>
         <bgColor rgb="0090EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF6347"/>
+        <bgColor rgb="00FF6347"/>
       </patternFill>
     </fill>
   </fills>
@@ -94,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -110,6 +117,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,12 +405,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40:$A$41</f>
+              <f>'Summary'!$A$40:$A$42</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40:$B$41</f>
+              <f>'Summary'!$B$40:$B$42</f>
             </numRef>
           </val>
         </ser>
@@ -522,6 +531,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -626,6 +638,36 @@
         <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2543175" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1002,7 +1044,16 @@
           <t>Vaishnavi</t>
         </is>
       </c>
-      <c r="G2" s="4" t="n"/>
+      <c r="F2" s="11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 17:03:01</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1381,20 +1432,6 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1504,7 +1541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1539,7 +1576,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1572,7 +1609,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1621,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Vaishnavi</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1633,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 10:17:01</t>
+          <t>2025-05-04 17:03:01</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1645,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[███-----------------] 16%</t>
+          <t>[████----------------] 22%</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1668,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1659,10 +1696,20 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>John</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1766,4 +1813,100 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Task 1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Home &gt; Login</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 17:03:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="12" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update by Vaishnavi on Task 1.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -40,7 +40,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +57,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ADD8E6"/>
         <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF6347"/>
+        <bgColor rgb="00FF6347"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -101,6 +107,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,6 +487,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400675" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -969,6 +1005,16 @@
           <t>Vaishnavi</t>
         </is>
       </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-05-04 21:34:27</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1236,7 +1282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1296,6 +1342,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1317,6 +1377,79 @@
       <c r="B21" s="6" t="inlineStr">
         <is>
           <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Task 1.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Home &gt; Login &gt; Username</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-04 21:34:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>Failed</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1500,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1400,7 +1533,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.1</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1557,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 21:33:47</t>
+          <t>2025-05-04 21:34:27</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1569,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[█-------------------] 5%</t>
+          <t>[██------------------] 11%</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1592,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1481,7 +1614,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update by Anmol on Task 4.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Task ID 2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Task ID 4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -293,12 +294,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Summary'!$A$20</f>
+              <f>'Summary'!$A$20:$A$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$20</f>
+              <f>'Summary'!$B$20:$B$21</f>
             </numRef>
           </val>
         </ser>
@@ -404,12 +405,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40:$A$41</f>
+              <f>'Summary'!$A$40:$A$42</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40:$B$41</f>
+              <f>'Summary'!$B$40:$B$42</f>
             </numRef>
           </val>
         </ser>
@@ -530,6 +531,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -634,6 +638,36 @@
         <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="942975" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1300,6 +1334,16 @@
           <t>Anmol</t>
         </is>
       </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-05-06 18:21:32</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
@@ -1394,20 +1438,6 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
@@ -1517,7 +1547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1542,7 +1572,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1573,7 +1603,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5.56%</t>
+          <t>11.11%</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1615,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1627,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vaishnavi</t>
+          <t>Anmol</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1639,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 21:51:19</t>
+          <t>2025-05-06 18:21:32</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1651,7 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>[███-----------------] 16%</t>
+          <t>[████----------------] 22%</t>
         </is>
       </c>
     </row>
@@ -1647,6 +1677,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
         <is>
@@ -1676,6 +1716,16 @@
         </is>
       </c>
       <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Anmol</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1779,4 +1829,100 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Task 4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Home&gt; Ai &gt;Integrate</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Anmol</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2025-05-06 18:21:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>